<commit_message>
tambah fitur upload siswa excel
</commit_message>
<xml_diff>
--- a/aplikasi/assets/template_siswa.xlsx
+++ b/aplikasi/assets/template_siswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\skripsi_lms\aplikasi\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219BE539-8A2B-4BC0-A7AB-CCA758F630A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66C8B64-486B-4A48-B267-34315D76A113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BD58EABA-1BD9-4BB6-B7CB-334394E76372}"/>
   </bookViews>
@@ -25,30 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>nis</t>
-  </si>
-  <si>
-    <t>nik</t>
-  </si>
-  <si>
-    <t>nama_siswa</t>
-  </si>
-  <si>
-    <t>alamat</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>kontak</t>
-  </si>
-  <si>
-    <t>kelas</t>
-  </si>
-  <si>
-    <t>nama_ibu</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>NIS</t>
+  </si>
+  <si>
+    <t>NIK</t>
+  </si>
+  <si>
+    <t>Nama_Siswa</t>
+  </si>
+  <si>
+    <t>Alamat</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Kontak</t>
+  </si>
+  <si>
+    <t>Kelas</t>
+  </si>
+  <si>
+    <t>Nama_Ibu</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -65,7 +68,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -409,41 +412,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B129CAFE-28EC-4168-B911-CF783367A848}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>